<commit_message>
fixed some errors after first run app
</commit_message>
<xml_diff>
--- a/data/trades_long.xlsx
+++ b/data/trades_long.xlsx
@@ -252,10 +252,10 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.09"/>
@@ -314,16 +314,16 @@
         <v>15</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>20000</v>
+        <v>18000</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>19800</v>
+        <v>17900</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>20200</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>0.01</v>
+        <v>0.001</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>20</v>

</xml_diff>